<commit_message>
added excel data file
</commit_message>
<xml_diff>
--- a/src/test/resources/SearchFoodItemFile.xlsx
+++ b/src/test/resources/SearchFoodItemFile.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="VERIFY_TABLE_DATA" sheetId="1" r:id="rId1"/>
+    <sheet name="Food_Item" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -16,24 +16,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>USERNAME</t>
+    <t>Food Item</t>
   </si>
   <si>
-    <t>PASSWORD</t>
+    <t>Fried Rice</t>
   </si>
   <si>
-    <t>T1</t>
-  </si>
-  <si>
-    <t>P1</t>
-  </si>
-  <si>
-    <t>T2</t>
-  </si>
-  <si>
-    <t>P2</t>
+    <t>Chicken Tandoori</t>
   </si>
 </sst>
 </file>
@@ -375,40 +366,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B4"/>
+  <dimension ref="A2:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>